<commit_message>
Refactor classes using includeFormat flag to use XLCellsUsedOptions instead.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/CopyingRowsAndColumns.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/CopyingRowsAndColumns.xlsx
@@ -423,10 +423,6 @@
       <x:c r="A2" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="F2" s="0" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:6">
-      <x:c r="F6" s="0" t="s"/>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="2">
@@ -446,7 +442,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:A6"/>
+  <x:dimension ref="A1:F6"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -501,7 +497,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:A8"/>
+  <x:dimension ref="A1:F8"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -591,16 +587,6 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:6">
-      <x:c r="B2" s="0" t="s"/>
-      <x:c r="D2" s="0" t="s"/>
-      <x:c r="F2" s="0" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:6">
-      <x:c r="B6" s="0" t="s"/>
-      <x:c r="D6" s="0" t="s"/>
-      <x:c r="F6" s="0" t="s"/>
-    </x:row>
   </x:sheetData>
   <x:mergeCells count="3">
     <x:mergeCell ref="B1:B6"/>
@@ -649,16 +635,6 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:6">
-      <x:c r="B2" s="0" t="s"/>
-      <x:c r="D2" s="0" t="s"/>
-      <x:c r="F2" s="0" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:6">
-      <x:c r="B6" s="0" t="s"/>
-      <x:c r="D6" s="0" t="s"/>
-      <x:c r="F6" s="0" t="s"/>
-    </x:row>
   </x:sheetData>
   <x:mergeCells count="3">
     <x:mergeCell ref="B1:B6"/>

</xml_diff>